<commit_message>
DG fragment prediction for [M+NH4]+.  Hunter Core changes
</commit_message>
<xml_diff>
--- a/ConfigurationFiles/02-Specific_ions_PL.xlsx
+++ b/ConfigurationFiles/02-Specific_ions_PL.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="95">
   <si>
     <t>PC</t>
   </si>
@@ -286,6 +286,24 @@
   </si>
   <si>
     <t>TG ammonium loss</t>
+  </si>
+  <si>
+    <t>NH3+H2O</t>
+  </si>
+  <si>
+    <t>TG ammonium loss + water</t>
+  </si>
+  <si>
+    <t>[M+H-H2O]+</t>
+  </si>
+  <si>
+    <t>H2O</t>
+  </si>
+  <si>
+    <t>TG water loss</t>
+  </si>
+  <si>
+    <t>DG</t>
   </si>
 </sst>
 </file>
@@ -654,10 +672,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1384,6 +1402,58 @@
         <v>88</v>
       </c>
     </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" s="1">
+        <v>35.037114000000003</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" s="1">
+        <v>18.010565</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>